<commit_message>
Working model - no PS constraints
</commit_message>
<xml_diff>
--- a/run_settings.xlsx
+++ b/run_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/maike_vanrooijen_wur_nl/Documents/05. PhD project/Paper 1; reducing householdfood waste by meal plans/Menu planning model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_F25DC773A252ABDACC10488821DF7E645ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44FF1FB3-2BCD-4B1B-8F4F-B7758C542AE2}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC10488821DF7E645ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E45BC373-9EB6-49D1-9F7B-5F604E8E05D7}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>n_days</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>run</t>
+  </si>
+  <si>
+    <t>DRVs</t>
+  </si>
+  <si>
+    <t>modelgezin_gemiddeld</t>
   </si>
 </sst>
 </file>
@@ -390,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,9 +407,10 @@
     <col min="2" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -419,8 +426,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -436,8 +446,11 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -453,8 +466,11 @@
       <c r="E3" t="s">
         <v>8</v>
       </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -470,8 +486,11 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -486,6 +505,9 @@
       </c>
       <c r="E5" t="s">
         <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add series run and testvariables (e.g. tvar1)
</commit_message>
<xml_diff>
--- a/run_settings.xlsx
+++ b/run_settings.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/maike_vanrooijen_wur_nl/Documents/05. PhD project/Paper 1; reducing householdfood waste by meal plans/Menu planning model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/maike_vanrooijen_wur_nl/Documents/05. PhD project/Paper 1; reducing householdfood waste by meal plans/3. Menu planning model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_F25DC773A252ABDACC10488821DF7E645ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E45BC373-9EB6-49D1-9F7B-5F604E8E05D7}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="11_F25DC773A252ABDACC10488821DF7E645ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61668A43-AA39-45EC-A865-4CC9E402E9F7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Stepwise_reduction_waste" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
   <si>
     <t>n_days</t>
   </si>
@@ -70,13 +71,52 @@
   </si>
   <si>
     <t>modelgezin_gemiddeld</t>
+  </si>
+  <si>
+    <t>run 5</t>
+  </si>
+  <si>
+    <t>run 6</t>
+  </si>
+  <si>
+    <t>run 7</t>
+  </si>
+  <si>
+    <t>run 8</t>
+  </si>
+  <si>
+    <t>run 9</t>
+  </si>
+  <si>
+    <t>run 10</t>
+  </si>
+  <si>
+    <t>run 11</t>
+  </si>
+  <si>
+    <t>run 12</t>
+  </si>
+  <si>
+    <t>run 13</t>
+  </si>
+  <si>
+    <t>run 14</t>
+  </si>
+  <si>
+    <t>run 15</t>
+  </si>
+  <si>
+    <t>run 16</t>
+  </si>
+  <si>
+    <t>tvar1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +128,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -398,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +487,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -461,7 +507,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -481,7 +527,7 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -501,7 +547,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -514,4 +560,418 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F72508C-10C4-4EC6-983B-E44464940A3E}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>0.1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>0.1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>0.1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>0.1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>0.1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add more analyses functions and series run
</commit_message>
<xml_diff>
--- a/run_settings.xlsx
+++ b/run_settings.xlsx
@@ -8,25 +8,39 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/maike_vanrooijen_wur_nl/Documents/05. PhD project/Paper 1; reducing householdfood waste by meal plans/3. Menu planning model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="11_F25DC773A252ABDACC10488821DF7E645ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61668A43-AA39-45EC-A865-4CC9E402E9F7}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="11_F25DC773A252ABDACC10488821DF7E645ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B67DE438-77B8-4224-9DBA-537FE7B53E5D}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Stepwise_reduction_waste" sheetId="2" r:id="rId2"/>
+    <sheet name="Stepwise_reduction_carbon" sheetId="3" r:id="rId3"/>
+    <sheet name="Household_size" sheetId="4" r:id="rId4"/>
+    <sheet name="All_objs" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="29">
   <si>
     <t>n_days</t>
   </si>
@@ -110,6 +124,9 @@
   </si>
   <si>
     <t>tvar1</t>
+  </si>
+  <si>
+    <t>Total_landuse</t>
   </si>
 </sst>
 </file>
@@ -445,7 +462,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F72508C-10C4-4EC6-983B-E44464940A3E}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,4 +991,847 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E631E4-76D7-4A77-903A-30EE29FBD124}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>29000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>28500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>27500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>26500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>0.1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>25500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>0.1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>24500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>0.1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13">
+        <v>23500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>0.1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>0.1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <v>21500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7C188A-695E-463F-9692-E52585082D1A}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>0.1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>0.1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>9999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2590A4A-541D-43AD-ABE1-05C410E1F1D8}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>0.1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6">
+        <v>9999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Long time no update
</commit_message>
<xml_diff>
--- a/run_settings.xlsx
+++ b/run_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/maike_vanrooijen_wur_nl/Documents/05. PhD project/Paper 1; reducing householdfood waste by meal plans/3. Menu planning model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="11_F25DC773A252ABDACC10488821DF7E645ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B67DE438-77B8-4224-9DBA-537FE7B53E5D}"/>
+  <xr:revisionPtr revIDLastSave="379" documentId="11_F25DC773A252ABDACC10488821DF7E645ADE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D93449F-C452-4B39-8AD3-4040A2A607CB}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Stepwise_reduction_carbon" sheetId="3" r:id="rId3"/>
     <sheet name="Household_size" sheetId="4" r:id="rId4"/>
     <sheet name="All_objs" sheetId="5" r:id="rId5"/>
+    <sheet name="wo_prev_recipes" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="71">
   <si>
     <t>n_days</t>
   </si>
@@ -127,6 +129,132 @@
   </si>
   <si>
     <t>Total_landuse</t>
+  </si>
+  <si>
+    <t>Pizza met courgette en sardientjes.txt</t>
+  </si>
+  <si>
+    <t>Stamppot boerenkool met makreel.txt</t>
+  </si>
+  <si>
+    <t>Tagliatelle met sardine-paprikasaus.txt</t>
+  </si>
+  <si>
+    <t>Ovenschotel voor de zaterdag.txt</t>
+  </si>
+  <si>
+    <t>Surinaamse nasi met boontjes en eierreepjes.txt</t>
+  </si>
+  <si>
+    <t>Rijst met sperziebonen (Lubia polo).txt</t>
+  </si>
+  <si>
+    <t>modelgezin_gemiddeld_gap</t>
+  </si>
+  <si>
+    <t>Stamppot rauwe andijvie met amandelen.txt</t>
+  </si>
+  <si>
+    <t>Tarwe met tomaatjes, noten en kruiden.txt</t>
+  </si>
+  <si>
+    <t>Venkel-radijssalade met walnoten en aardappelpuree.txt</t>
+  </si>
+  <si>
+    <t>Linzenburger met pikante wortelsalade.txt</t>
+  </si>
+  <si>
+    <t>Stoofpot met pastinaak en witte bonen.txt</t>
+  </si>
+  <si>
+    <t>Ravioli met paddenstoelen en noten.txt</t>
+  </si>
+  <si>
+    <t>Bulgur met groente, tofu en noten.txt</t>
+  </si>
+  <si>
+    <t>Spinazie-ovenschotel.txt</t>
+  </si>
+  <si>
+    <t>Andijviestamppot met champignons en tofu-notenkruim.txt</t>
+  </si>
+  <si>
+    <t>Drie bonensalade.txt</t>
+  </si>
+  <si>
+    <t>Tortilla met gekaramelliseerde uien.txt</t>
+  </si>
+  <si>
+    <t>Pittige Chinese kool.txt</t>
+  </si>
+  <si>
+    <t>Notenrijst met aubergine.txt</t>
+  </si>
+  <si>
+    <t>Penne met romige spinazie en zalm.txt</t>
+  </si>
+  <si>
+    <t>Maaltijd-pastasalade met tomaatjes.txt</t>
+  </si>
+  <si>
+    <t>Aardappeltaart met rozemarijn en komkommer-radijssalade.txt</t>
+  </si>
+  <si>
+    <t>Kruidige rijst met tofu en abrikozen.txt</t>
+  </si>
+  <si>
+    <t>Kruidig roerei.txt</t>
+  </si>
+  <si>
+    <t>Pizza.txt</t>
+  </si>
+  <si>
+    <t>Penne met tonijn en roerbakgroente.txt</t>
+  </si>
+  <si>
+    <t>Spaghetti met venkel-uiensaus en noten.txt</t>
+  </si>
+  <si>
+    <t>Penne met champignons, tomaatjes en oregano.txt</t>
+  </si>
+  <si>
+    <t>Pizza van Turks brood met sardientjes.txt</t>
+  </si>
+  <si>
+    <t>Farro met geroosterde groente en noten.txt</t>
+  </si>
+  <si>
+    <t>Franse uientaart.txt</t>
+  </si>
+  <si>
+    <t>Bruine bonensoep.txt</t>
+  </si>
+  <si>
+    <t>Bulgursalade met sperzieboontjes en cashewnoten.txt</t>
+  </si>
+  <si>
+    <t>Courgettefritters.txt</t>
+  </si>
+  <si>
+    <t>Gestoofde kabeljauw met snijbonen.txt</t>
+  </si>
+  <si>
+    <t>Geroerbakte biefstuk.txt</t>
+  </si>
+  <si>
+    <t>De drie gezusters.txt</t>
+  </si>
+  <si>
+    <t>Erwtensoep (Snert).txt</t>
+  </si>
+  <si>
+    <t>Pasta met noten en olijven.txt</t>
+  </si>
+  <si>
+    <t>Gekaramelliseerde tomaatjes met witte bonenpuree en paddenstoelen.txt</t>
+  </si>
+  <si>
+    <t>Tostada met driebonensalade.txt</t>
   </si>
 </sst>
 </file>
@@ -164,10 +292,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -176,9 +313,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +600,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +648,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -581,10 +719,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F72508C-10C4-4EC6-983B-E44464940A3E}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G6"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,10 +730,10 @@
     <col min="2" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -618,7 +756,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -629,19 +767,19 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G2">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -652,19 +790,20 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G3">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <f>G2-$J$5</f>
+        <v>945</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -675,19 +814,20 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G4">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G4:G11" si="0">G3-$J$5</f>
+        <v>840</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -698,19 +838,24 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G5">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>735</v>
+      </c>
+      <c r="J5">
+        <f>1050/10</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -721,19 +866,20 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G6">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -744,19 +890,20 @@
         <v>4</v>
       </c>
       <c r="D7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G7">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -767,19 +914,20 @@
         <v>4</v>
       </c>
       <c r="D8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G8">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -790,19 +938,20 @@
         <v>4</v>
       </c>
       <c r="D9">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G9">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -813,19 +962,20 @@
         <v>4</v>
       </c>
       <c r="D10">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G10">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -836,19 +986,24 @@
         <v>4</v>
       </c>
       <c r="D11">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G11">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="J11">
+        <f>G11/6</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -859,19 +1014,20 @@
         <v>4</v>
       </c>
       <c r="D12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G12">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <f>G11-$J$11</f>
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -882,19 +1038,20 @@
         <v>4</v>
       </c>
       <c r="D13">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G13">
+        <f t="shared" ref="G13:G16" si="1">G12-$J$11</f>
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -905,19 +1062,20 @@
         <v>4</v>
       </c>
       <c r="D14">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G14">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -928,19 +1086,20 @@
         <v>4</v>
       </c>
       <c r="D15">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G15">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -951,16 +1110,17 @@
         <v>4</v>
       </c>
       <c r="D16">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G16">
-        <v>40</v>
+        <f t="shared" si="1"/>
+        <v>17.5</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -974,16 +1134,16 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G17">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -997,8 +1157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E631E4-76D7-4A77-903A-30EE29FBD124}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1202,7 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -1065,7 +1225,7 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1088,7 +1248,7 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -1111,7 +1271,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -1134,7 +1294,7 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -1157,7 +1317,7 @@
         <v>4</v>
       </c>
       <c r="D7">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -1180,7 +1340,7 @@
         <v>4</v>
       </c>
       <c r="D8">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -1203,7 +1363,7 @@
         <v>4</v>
       </c>
       <c r="D9">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -1226,7 +1386,7 @@
         <v>4</v>
       </c>
       <c r="D10">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -1249,7 +1409,7 @@
         <v>4</v>
       </c>
       <c r="D11">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -1272,7 +1432,7 @@
         <v>4</v>
       </c>
       <c r="D12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -1295,7 +1455,7 @@
         <v>4</v>
       </c>
       <c r="D13">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -1318,7 +1478,7 @@
         <v>4</v>
       </c>
       <c r="D14">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -1341,7 +1501,7 @@
         <v>4</v>
       </c>
       <c r="D15">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -1364,7 +1524,7 @@
         <v>4</v>
       </c>
       <c r="D16">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
@@ -1387,7 +1547,7 @@
         <v>4</v>
       </c>
       <c r="D17">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -1682,8 +1842,166 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2590A4A-541D-43AD-ABE1-05C410E1F1D8}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6">
+        <v>9999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385617EB-FECF-4EF2-892D-D7986C213B4D}">
+  <dimension ref="A1:Q6"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,9 +2009,11 @@
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1716,7 +2036,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1727,19 +2047,50 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="G2" t="str">
+        <f>_xlfn.TEXTJOIN(";",TRUE,wo_prev_recipes!H2:Q2)</f>
+        <v>Stamppot rauwe andijvie met amandelen.txt;Tarwe met tomaatjes, noten en kruiden.txt;Venkel-radijssalade met walnoten en aardappelpuree.txt;Linzenburger met pikante wortelsalade.txt;Stoofpot met pastinaak en witte bonen.txt;Farro met geroosterde groente en noten.txt;Franse uientaart.txt;Bruine bonensoep.txt;Bulgursalade met sperzieboontjes en cashewnoten.txt;Drie bonensalade.txt</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1750,19 +2101,50 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="G3" t="str">
+        <f>_xlfn.TEXTJOIN(";",TRUE,wo_prev_recipes!H3:Q3)</f>
+        <v>Tagliatelle met sardine-paprikasaus.txt;Stamppot boerenkool met makreel.txt;Ovenschotel voor de zaterdag.txt;Pizza met courgette en sardientjes.txt;Notenrijst met aubergine.txt;Pizza.txt;Penne met tonijn en roerbakgroente.txt;Spaghetti met venkel-uiensaus en noten.txt;Penne met champignons, tomaatjes en oregano.txt;Pizza van Turks brood met sardientjes.txt</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N3" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1773,19 +2155,50 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="G4" t="str">
+        <f>_xlfn.TEXTJOIN(";",TRUE,wo_prev_recipes!H4:Q4)</f>
+        <v>Tarwe met tomaatjes, noten en kruiden.txt;Ravioli met paddenstoelen en noten.txt;Bulgur met groente, tofu en noten.txt;Spinazie-ovenschotel.txt;Andijviestamppot met champignons en tofu-notenkruim.txt;Penne met romige spinazie en zalm.txt;Maaltijd-pastasalade met tomaatjes.txt;Aardappeltaart met rozemarijn en komkommer-radijssalade.txt;Kruidige rijst met tofu en abrikozen.txt;Kruidig roerei.txt</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1796,19 +2209,50 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="G5" t="str">
+        <f>_xlfn.TEXTJOIN(";",TRUE,wo_prev_recipes!H5:Q5)</f>
+        <v>Bulgur met groente, tofu en noten.txt;Spinazie-ovenschotel.txt;Tarwe met tomaatjes, noten en kruiden.txt;Ravioli met paddenstoelen en noten.txt;Andijviestamppot met champignons en tofu-notenkruim.txt;Courgettefritters.txt;Kruidig roerei.txt;Gestoofde kabeljauw met snijbonen.txt;Geroerbakte biefstuk.txt;Bulgursalade met sperzieboontjes en cashewnoten.txt</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1819,19 +2263,62 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6">
-        <v>9999</v>
+        <v>35</v>
+      </c>
+      <c r="G6" t="str">
+        <f>_xlfn.TEXTJOIN(";",TRUE,wo_prev_recipes!H6:Q6)</f>
+        <v>Drie bonensalade.txt;Tortilla met gekaramelliseerde uien.txt;Surinaamse nasi met boontjes en eierreepjes.txt;Rijst met sperziebonen (Lubia polo).txt;Pittige Chinese kool.txt;De drie gezusters.txt;Erwtensoep (Snert).txt;Pasta met noten en olijven.txt;Gekaramelliseerde tomaatjes met witte bonenpuree en paddenstoelen.txt;Tostada met driebonensalade.txt</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" t="s">
+        <v>67</v>
+      </c>
+      <c r="O6" t="s">
+        <v>68</v>
+      </c>
+      <c r="P6" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2A84F0-55DE-45F0-996E-1DF6D1BD28C6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>